<commit_message>
feat: Update UI and texts for v1.0.1 release
</commit_message>
<xml_diff>
--- a/public/images/UI versions.xlsx
+++ b/public/images/UI versions.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\Booktok\booktok-frontend\public\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{209B7297-46F3-4A69-AD01-C5C43E879654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D62F3D08-E51E-46E2-A7B5-1C6E6CE28A9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="input" sheetId="1" r:id="rId1"/>
+    <sheet name="loading" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -85,14 +86,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>4380</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>313658</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>309278</xdr:colOff>
       <xdr:row>48</xdr:row>
       <xdr:rowOff>103294</xdr:rowOff>
     </xdr:to>
@@ -129,13 +130,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>355372</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>523875</xdr:colOff>
       <xdr:row>47</xdr:row>
       <xdr:rowOff>176432</xdr:rowOff>
@@ -173,13 +174,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>392141</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>438150</xdr:colOff>
       <xdr:row>47</xdr:row>
       <xdr:rowOff>75791</xdr:rowOff>
@@ -207,6 +208,231 @@
         <a:xfrm>
           <a:off x="9993341" y="647700"/>
           <a:ext cx="2789209" cy="7933916"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>391132</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>161926</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="图片 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA5076D4-129A-3C0C-DB05-37088B3FCD1A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12877800" y="762001"/>
+          <a:ext cx="2600932" cy="5010150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>352426</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>63117</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="图片 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DB3069D-745F-2C35-A29F-8392DD11A113}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15440026" y="762000"/>
+          <a:ext cx="2453891" cy="5781675"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>133351</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>43247</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="图片 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E2231FA-B606-69BC-5817-BE24BF4FF38A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17811750" y="676276"/>
+          <a:ext cx="2805497" cy="5924550"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>427562</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="图片 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79C3F81E-F003-F6C7-2867-DA03B0B66ADF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16392525" y="733425"/>
+          <a:ext cx="2551637" cy="5857875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>577097</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>151283</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="图片 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A42367ED-598C-4E1D-83E5-6EEC293E9F4A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1009650" y="723900"/>
+          <a:ext cx="2996447" cy="6123458"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -483,8 +709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U38" sqref="U38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AC40" sqref="AC40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -493,4 +719,21 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92494024-5E06-4E10-B326-14B8953F91B5}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>